<commit_message>
TestTask - Fixed bug and refactoring:    - Add generic classes "...Importer/...Export/Sheet..."    - Rename classes and property    - Fixed bug Import file    - Remove unused code    - Transition from "enum" to "SmartEnum"
</commit_message>
<xml_diff>
--- a/TestTask.Test/Resources/ColumnNameIsNotCorrect.xlsx
+++ b/TestTask.Test/Resources/ColumnNameIsNotCorrect.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\TASK\TestTask.Data\22.11.2023_22-45\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\TestTask\TestTask.Test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60454519-AC6A-42E6-AF64-A646B1F653B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CBD100-80F3-4627-B409-28EB7469F023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
     <sheet name="Product" sheetId="2" r:id="rId2"/>
     <sheet name="Category" sheetId="3" r:id="rId3"/>
-    <sheet name="Type" sheetId="4" r:id="rId4"/>
+    <sheet name="ProductType" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -460,7 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -663,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TestTask - Fixed bug and refactoring (#134)
* TestTask - Fixed bug and refactoring:
   - Add generic classes "...Importer/...Export/Sheet..."
   - Rename classes and property
   - Fixed bug Import file
   - Remove unused code
   - Transition from "enum" to "SmartEnum"

* TestTask - Add folder
</commit_message>
<xml_diff>
--- a/TestTask.Test/Resources/ColumnNameIsNotCorrect.xlsx
+++ b/TestTask.Test/Resources/ColumnNameIsNotCorrect.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\TASK\TestTask.Data\22.11.2023_22-45\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\TestTask\TestTask.Test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60454519-AC6A-42E6-AF64-A646B1F653B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CBD100-80F3-4627-B409-28EB7469F023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
     <sheet name="Product" sheetId="2" r:id="rId2"/>
     <sheet name="Category" sheetId="3" r:id="rId3"/>
-    <sheet name="Type" sheetId="4" r:id="rId4"/>
+    <sheet name="ProductType" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -460,7 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -663,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>